<commit_message>
Updated the dataProvider method to read data from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -43,24 +43,6 @@
   </si>
   <si>
     <t>Zohoautomation@1</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>QEW</t>
-  </si>
-  <si>
-    <t>SFAD</t>
-  </si>
-  <si>
-    <t>DFFV</t>
-  </si>
-  <si>
-    <t>EWREQ</t>
-  </si>
-  <si>
-    <t>SAFADS</t>
   </si>
 </sst>
 </file>
@@ -378,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -390,59 +372,36 @@
     <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>